<commit_message>
added some data for preliminary results. added code to process the data
</commit_message>
<xml_diff>
--- a/data_analysis/WS950_WZ90_p15_t10.xlsx
+++ b/data_analysis/WS950_WZ90_p15_t10.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix Neubürger\sciebo\WiTraPres\Daten\FEM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix Neubürger\Documents\GitHub\CoupledFEMSimulations\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -104,9 +104,6 @@
     <t>Zarge oben</t>
   </si>
   <si>
-    <t>Timestamp</t>
-  </si>
-  <si>
     <t>Stempel_innen_mitte</t>
   </si>
   <si>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>Werkstueck_zarge_oben</t>
+  </si>
+  <si>
+    <t>timestamp</t>
   </si>
 </sst>
 </file>
@@ -4217,7 +4217,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8094,7 +8093,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9610,7 +9608,7 @@
   <dimension ref="A1:K300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9629,37 +9627,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>33</v>
-      </c>
-      <c r="K1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>